<commit_message>
updating with CE activities
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Continuing Eductation" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
   <si>
     <t>Title</t>
   </si>
@@ -151,6 +151,114 @@
   </si>
   <si>
     <t>International Society of Exposure Science 25th Annual Meeting</t>
+  </si>
+  <si>
+    <t>San Diego, CA</t>
+  </si>
+  <si>
+    <t>American Society of Safety Engineers</t>
+  </si>
+  <si>
+    <t>Conducting a Safety Audit</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Georgia Public Safety Training Center</t>
+  </si>
+  <si>
+    <t>Basic Course for Health Assessment and Consultation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency for Toxic Substances and Disease Registry </t>
+  </si>
+  <si>
+    <t>Introduction to Risk Assessment Guidance for Superfund</t>
+  </si>
+  <si>
+    <t>US Environmental Protection Agency</t>
+  </si>
+  <si>
+    <t>Time Series and Forecasting</t>
+  </si>
+  <si>
+    <t>Practical Stats, Inc.</t>
+  </si>
+  <si>
+    <t>Untangling Multivariate Relationships</t>
+  </si>
+  <si>
+    <t>Nondetects and Data Analysis, Statistical Methods for Censored Environmental Data</t>
+  </si>
+  <si>
+    <t>Principles of Quality Assurance and Quality Control in Environmental Field Programs</t>
+  </si>
+  <si>
+    <t>Montgomery, AL</t>
+  </si>
+  <si>
+    <t>Northwest Environmental Training Center</t>
+  </si>
+  <si>
+    <t>Exposure Risk Training</t>
+  </si>
+  <si>
+    <t>US Environmental Protection Agency Office of Air Quality Planning and Standards</t>
+  </si>
+  <si>
+    <t>Intermediate Incident Command System for Expanding Incidents (ICS300)</t>
+  </si>
+  <si>
+    <t>US Centers for Disease Control and Prevention</t>
+  </si>
+  <si>
+    <t>Applied Environmental Statistics</t>
+  </si>
+  <si>
+    <t>Advanced Command System for Command and General Staff, Complex Incidents and MACS (ICS400)</t>
+  </si>
+  <si>
+    <t>Sampling for Hazardous Matrials</t>
+  </si>
+  <si>
+    <t>Air Monitoring for Emergency Response</t>
+  </si>
+  <si>
+    <t>Interpretation of Biomonitoring Data using Physiologically Based Pharmokinetic (PBPK) Modeling</t>
+  </si>
+  <si>
+    <t>RTP, NC</t>
+  </si>
+  <si>
+    <t>Environmental Sampling, Sampling Reliability and Data Quality Objectives for the Health Assessment Process</t>
+  </si>
+  <si>
+    <t>Envirostat, Inc.</t>
+  </si>
+  <si>
+    <t>CIIT Centers for Health Research</t>
+  </si>
+  <si>
+    <t>AERMOD Air Dispersion Modeling</t>
+  </si>
+  <si>
+    <t>Chicago, IL</t>
+  </si>
+  <si>
+    <t>Lakes Environmental</t>
+  </si>
+  <si>
+    <t>Edison, NJ</t>
+  </si>
+  <si>
+    <t>Health and Safety (40 Hour HAZWOPER)</t>
+  </si>
+  <si>
+    <t>Longmont, CO</t>
+  </si>
+  <si>
+    <t>\\cdc.gov\private\M309\Hzd3\training\Certificates</t>
   </si>
 </sst>
 </file>
@@ -469,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +642,367 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1">
+        <v>36617</v>
+      </c>
+      <c r="C3" s="1">
+        <v>36617</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40241</v>
+      </c>
+      <c r="C4" s="1">
+        <v>405483</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1">
+        <v>40805</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40809</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41345</v>
+      </c>
+      <c r="C6" s="1">
+        <v>41347</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41345</v>
+      </c>
+      <c r="C7" s="1">
+        <v>41346</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1">
+        <v>40982</v>
+      </c>
+      <c r="C8" s="1">
+        <v>40983</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1">
+        <v>40771</v>
+      </c>
+      <c r="C9" s="1">
+        <v>40772</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1">
+        <v>40277</v>
+      </c>
+      <c r="C10" s="1">
+        <v>40278</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42234</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42236</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="1">
+        <v>40118</v>
+      </c>
+      <c r="C12" s="1">
+        <v>40120</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1">
+        <v>40287</v>
+      </c>
+      <c r="C13" s="1">
+        <v>40291</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1">
+        <v>39322</v>
+      </c>
+      <c r="C14" s="1">
+        <v>39324</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="1">
+        <v>38880</v>
+      </c>
+      <c r="C15" s="1">
+        <v>38881</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="1">
+        <v>38985</v>
+      </c>
+      <c r="C16" s="1">
+        <v>38989</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="1">
+        <v>39629</v>
+      </c>
+      <c r="C17" s="1">
+        <v>39632</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="1">
+        <v>39352</v>
+      </c>
+      <c r="C18" s="1">
+        <v>39353</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1">
+        <v>39818</v>
+      </c>
+      <c r="C19" s="1">
+        <v>39822</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -543,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating with more information.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hzd3\gitlab\cv_jim\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB351372-8E11-4F47-87B2-5BDB283B1CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="2835" yWindow="1455" windowWidth="20145" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Continuing Eductation" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="131">
   <si>
     <t>Title</t>
   </si>
@@ -259,19 +260,188 @@
   </si>
   <si>
     <t>\\cdc.gov\private\M309\Hzd3\training\Certificates</t>
+  </si>
+  <si>
+    <t>CDC Statistics Day</t>
+  </si>
+  <si>
+    <t>Characterization of particulate matter (PM10) from Beta Attenuation Monitor and Partisol sampler at Valley School, Washington using openair package for R statistical software</t>
+  </si>
+  <si>
+    <t>Geological Society of America</t>
+  </si>
+  <si>
+    <t>Charlotte, NC</t>
+  </si>
+  <si>
+    <t>Geology and Health Insights Into Lead Poisoning From Artisanal Gold Mining, NW Nigeria: Sources, Exposure Pathways, Additional Health Concerns, and Global Implications.</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Lead Poisoning Outbreak Zamfara State, Nigeria 2010 – Public Health and Geochemical Investigations</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Florence, AL</t>
+  </si>
+  <si>
+    <t>AmericanChemicalSociety Wilson Dam Section
+Univ. North Alabama American Industrial Hygiene Association Student Section</t>
+  </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topics in Environmental Exposure Investigation </t>
+  </si>
+  <si>
+    <t>Analysis of Environmental Data - Censored Data Demythed</t>
+  </si>
+  <si>
+    <t>Ethylene Oxide Air Monitoring Data Analysis Sterigenics International Facility – Willowbrook, IL</t>
+  </si>
+  <si>
+    <t>Georgia Local Section, American Industrial Hygiene Association</t>
+  </si>
+  <si>
+    <t>Stats, R</t>
+  </si>
+  <si>
+    <t>Stats, R, Air</t>
+  </si>
+  <si>
+    <t>Exposure Point Concentration (EPC) Guidance Development - A Sneak Peek at What is Coming!</t>
+  </si>
+  <si>
+    <t>J. Durant, G. Ulirsch</t>
+  </si>
+  <si>
+    <t>Stats, Policy</t>
+  </si>
+  <si>
+    <t>ATSDR’s Partnership to Promote Localized Efforts to Reduce Environmental Exposure (APPLETREE) Partners Meeting</t>
+  </si>
+  <si>
+    <t>G. Plumlee ,J. Durant</t>
+  </si>
+  <si>
+    <t>Technical Assistance Report: Characterization of particulate matter (PM10) from Beta Attenuation Monitor and Partisol sampler at Valley School, Washington using openair package for R statistical software</t>
+  </si>
+  <si>
+    <t>ATSDR</t>
+  </si>
+  <si>
+    <t>The openair package: Tools for data analysis of air contaminants using R</t>
+  </si>
+  <si>
+    <t>ATSDR Topics in Exposure Investigations</t>
+  </si>
+  <si>
+    <t>B. Goodwin, D. Gable, A. Young, J. Durant</t>
+  </si>
+  <si>
+    <t>Exposure Investigation: Airborne Exposures to Particulate Matter and Silica Dust in Valley School, Valley, WA</t>
+  </si>
+  <si>
+    <t>Exposure Investigation: DuPont Delisle Plant, Pass Christian, Harrison county, MS</t>
+  </si>
+  <si>
+    <t>Dioxin</t>
+  </si>
+  <si>
+    <t>J. Durant L. Rosales-Guevara, G. Zarus</t>
+  </si>
+  <si>
+    <t>Exposure Investigation: Illinois Beach State Park, Zion, Lake County, IL</t>
+  </si>
+  <si>
+    <t>J. Durant J. Wheeler, M Johnson</t>
+  </si>
+  <si>
+    <t>Asbestos</t>
+  </si>
+  <si>
+    <t>Addendum to the Toxicological Profile for 3,3’-Dichlorobenzidine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J. Durant, Y. Iossifova, J. Purvis </t>
+  </si>
+  <si>
+    <t>Tox</t>
+  </si>
+  <si>
+    <t>Health Consultation – Sulfolane (I)</t>
+  </si>
+  <si>
+    <t>Health Consultation – Sulfolane (II)</t>
+  </si>
+  <si>
+    <t>Community Meeting - Sulfolane Public Health Consultation</t>
+  </si>
+  <si>
+    <t>North Pole, AK</t>
+  </si>
+  <si>
+    <t>Alaska Department of Health Environmental Public Health Program</t>
+  </si>
+  <si>
+    <t>Poster Session: 	Exposure Investigation of Asbestos in the Sands of Illinois Beach State Park</t>
+  </si>
+  <si>
+    <t>J. Durant, J. Wheeler, M. Johnson, S. Metcalf</t>
+  </si>
+  <si>
+    <t>Altanta, GA</t>
+  </si>
+  <si>
+    <t>National Environmental Public Health Conference</t>
+  </si>
+  <si>
+    <t>How to Handle Non-detect Environmental Data? Kaplan-Meier Product Limit and Alternatives</t>
+  </si>
+  <si>
+    <t>Atlanta,GA</t>
+  </si>
+  <si>
+    <t>ATSDR Office of Community Health Hazard Assessment Brown Bag</t>
+  </si>
+  <si>
+    <t>Health Consultation: Pointe Coupee Wood Treating, New Roads, Point Couppe Parish, LA</t>
+  </si>
+  <si>
+    <t>J. Durant, SC Tsai</t>
+  </si>
+  <si>
+    <t>Health Consultation: Burlington Northern Fueling Facility, Helena, MT</t>
+  </si>
+  <si>
+    <t>Health Consultation: Review of Analysis of Particulate Matter and Metal Exposures in Air, KCBX, Chicago, Cook County, IL</t>
+  </si>
+  <si>
+    <t>M. Colledge, J. Durant, B. Goodwin, M. Caudill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -294,9 +464,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,10 +747,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1005,15 +1176,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,25 +1473,519 @@
         <v>40</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1">
+        <v>41878</v>
+      </c>
+      <c r="D13" s="1">
+        <v>41878</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="1">
+        <v>41219</v>
+      </c>
+      <c r="D14" s="1">
+        <v>41219</v>
+      </c>
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1">
+        <v>41753</v>
+      </c>
+      <c r="D15" s="1">
+        <v>41753</v>
+      </c>
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43181</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43181</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43776</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43776</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="1">
+        <v>42872</v>
+      </c>
+      <c r="D18" s="1">
+        <v>42872</v>
+      </c>
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1">
+        <v>42789</v>
+      </c>
+      <c r="D19" s="1">
+        <v>42789</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1">
+        <v>40680</v>
+      </c>
+      <c r="D20" s="1">
+        <v>40680</v>
+      </c>
+      <c r="E20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="1">
+        <v>40112</v>
+      </c>
+      <c r="D21" s="1">
+        <v>40112</v>
+      </c>
+      <c r="E21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44783</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44783</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1">
+        <v>41965</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41965</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43676</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43676</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="1">
+        <v>39176</v>
+      </c>
+      <c r="D4" s="1">
+        <v>39176</v>
+      </c>
+      <c r="E4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="1">
+        <v>39374</v>
+      </c>
+      <c r="D5" s="1">
+        <v>39374</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="1">
+        <v>40299</v>
+      </c>
+      <c r="D6" s="1">
+        <v>40299</v>
+      </c>
+      <c r="E6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1">
+        <v>40665</v>
+      </c>
+      <c r="D7" s="1">
+        <v>40665</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>40212</v>
+      </c>
+      <c r="D8" s="1">
+        <v>40212</v>
+      </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1">
+        <v>38134</v>
+      </c>
+      <c r="D9" s="1">
+        <v>38134</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="1">
+        <v>38723</v>
+      </c>
+      <c r="D10" s="1">
+        <v>38723</v>
+      </c>
+      <c r="E10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42604</v>
+      </c>
+      <c r="D11" s="1">
+        <v>42604</v>
+      </c>
+      <c r="E11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1329,11 +1995,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1341,5 +2008,6 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>